<commit_message>
Added user stories for sprint 5
</commit_message>
<xml_diff>
--- a/UserStories/output.xlsx
+++ b/UserStories/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,236 +424,187 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Wireframes and Mockups for Unified Operations Dashboard for Managers</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>As a Product Team, we need wireframes and mockups for the 'Unified Operations Dashboard for Managers' so that managers have a cohesive, intuitive, and user-centric experience from day one.</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Acceptance Criteria 1</t>
+          <t>GIVEN a manager logs in, WHEN they view their dashboard, THEN all core modules are presented clearly and intuitively.
+GIVEN a user views any screen, WHEN they interact with it, THEN the design is consistent with the established brand and style guide.</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Acceptance Criteria 2</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Priority</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Story Points</t>
+          <t>None specified</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Dependencies</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Notes</t>
+          <t>Scope limited to wireframes and mockups for the Unified Operations Dashboard for Managers.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Design Unified Operations Dashboard for Managers</t>
+          <t>Design for Integrated Incident Reporting Form and Submission Flow</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>As a manager, I want a unified operations dashboard with clear and intuitive modules so that I can efficiently oversee all core platform features from a single view.</t>
+          <t>As a Product Team, we need the design for the 'Integrated Incident Reporting' form and submission flow so that staff can report incidents simply, quickly, and with minimal training.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GIVEN a manager logs in, WHEN they view their dashboard, THEN all core modules (Operations, Incident Reporting, Staff Schedule, Compliance Tracking) are presented clearly and intuitively.</t>
+          <t>GIVEN a staff member needs to report an incident, WHEN they access the form, THEN the process is simple, quick, and requires minimal training.
+GIVEN a user views any screen, WHEN they interact with it, THEN the design is consistent with the established brand and style guide.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GIVEN a manager interacts with any dashboard module, WHEN they navigate between modules, THEN the design remains consistent with the established brand and style guide.</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Wireframes and mockups must be reviewed by the Product Team and validated against the style guide.</t>
+          <t>None specified</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Scope limited to the design and submission flow for the Integrated Incident Reporting form.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Design Integrated Incident Reporting Form and Submission Flow</t>
+          <t>UI for Staff Task &amp; Schedule Viewer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>As a staff member, I want an integrated incident reporting form with a simple and quick submission flow so that I can report incidents efficiently with minimal training.</t>
+          <t>As a Product Team, we need the UI for the 'Staff Task &amp; Schedule Viewer' so that staff can intuitively view their tasks and schedules.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GIVEN a staff member needs to report an incident, WHEN they access the incident reporting form, THEN the process is simple, quick, and requires minimal training.</t>
+          <t>GIVEN a user views any screen, WHEN they interact with it, THEN the design is consistent with the established brand and style guide.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GIVEN a user interacts with the incident reporting form, WHEN they submit a report, THEN the design and flow are consistent with the established brand and style guide.</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Design should be validated with user testing for intuitiveness and speed.</t>
+          <t>None specified</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Scope limited to the UI for the Staff Task &amp; Schedule Viewer.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Design Staff Task &amp; Schedule Viewer UI</t>
+          <t>Visual Design for Compliance &amp; Certification Tracking Module</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>As a staff member, I want a clear and intuitive UI for viewing my tasks and schedule so that I can easily manage my responsibilities.</t>
+          <t>As a Product Team, we need the visual design for the 'Compliance &amp; Certification Tracking' module so that users can track compliance and certifications within a cohesive and branded interface.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GIVEN a staff member logs in, WHEN they view the task &amp; schedule viewer, THEN all relevant information is presented clearly and intuitively.</t>
+          <t>GIVEN a user views any screen, WHEN they interact with it, THEN the design is consistent with the established brand and style guide.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GIVEN a user interacts with the schedule viewer, WHEN they navigate or filter tasks, THEN the design is consistent with the established brand and style guide.</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>UI should support filtering and sorting of tasks; must be reviewed for accessibility.</t>
+          <t>None specified</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Scope limited to the visual design for the Compliance &amp; Certification Tracking module.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Visual Design for Compliance &amp; Certification Tracking Module</t>
+          <t>User Flow Mapping for Closed-Loop Incident-to-Training Workflow</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>As a compliance officer, I want a visually clear and branded module for tracking compliance and certifications so that I can monitor and manage regulatory requirements efficiently.</t>
+          <t>As a Product Team, we need user flow mapping for the 'Closed-Loop Incident-to-Training Workflow' so that the process from incident reporting to training is clearly defined and user-centric.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>GIVEN a user accesses the compliance &amp; certification tracking module, WHEN they view compliance statuses, THEN information is presented clearly and intuitively.</t>
+          <t>GIVEN a user views any screen, WHEN they interact with it, THEN the design is consistent with the established brand and style guide.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GIVEN a user interacts with the module, WHEN they perform actions (e.g., update status), THEN the design is consistent with the established brand and style guide.</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Not specified</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Visual design must be reviewed by compliance stakeholders for accuracy and clarity.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Map User Flow for Closed-Loop Incident-to-Training Workflow</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>As a training coordinator, I want a mapped user flow for the closed-loop incident-to-training workflow so that incidents can be seamlessly linked to relevant training interventions.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GIVEN an incident is reported, WHEN the workflow triggers a training requirement, THEN the user flow is clear, intuitive, and consistent with the established brand and style guide.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>GIVEN a user completes a training linked to an incident, WHEN they view the workflow status, THEN the process is visually clear and easy to follow.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Incident Reporting Form Design</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>User flow mapping should be validated with end-to-end user testing.</t>
+          <t>None specified</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Scope limited to user flow mapping for the Closed-Loop Incident-to-Training Workflow.</t>
         </is>
       </c>
     </row>

</xml_diff>